<commit_message>
Improve to 74.86% accuracy Experience_Classification
</commit_message>
<xml_diff>
--- a/Test_Results_Translated_Experience.xlsx
+++ b/Test_Results_Translated_Experience.xlsx
@@ -632,10 +632,8 @@
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G7" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -659,10 +657,8 @@
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1030,10 +1026,8 @@
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1700,10 +1694,8 @@
       </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G45" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1727,10 +1719,8 @@
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2005,10 +1995,8 @@
       </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G56" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2119,10 +2107,8 @@
       </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G60" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="61">
@@ -2222,17 +2208,13 @@
           <t>Bachelor's Degree</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="D64" t="n">
+        <v>0</v>
       </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">

</xml_diff>

<commit_message>
Improve to 85.14% accuracy Experience_Classification
</commit_message>
<xml_diff>
--- a/Test_Results_Translated_Experience.xlsx
+++ b/Test_Results_Translated_Experience.xlsx
@@ -632,8 +632,10 @@
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>10</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -1609,10 +1611,8 @@
       </c>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G42" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="43">
@@ -2107,8 +2107,10 @@
       </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr"/>
-      <c r="G60" t="n">
-        <v>10</v>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
       </c>
     </row>
     <row r="61">
@@ -2292,10 +2294,8 @@
       </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G67" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -2777,10 +2777,8 @@
       </c>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr"/>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G84" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -2804,10 +2802,8 @@
       </c>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G85" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -2831,10 +2827,8 @@
       </c>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G86" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -2859,7 +2853,7 @@
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -2941,10 +2935,8 @@
       </c>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G90" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -2997,10 +2989,8 @@
       </c>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G92" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="93">
@@ -3132,10 +3122,8 @@
       </c>
       <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr"/>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G97" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="98">
@@ -3325,10 +3313,8 @@
       </c>
       <c r="E104" t="inlineStr"/>
       <c r="F104" t="inlineStr"/>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G104" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="105">
@@ -3661,10 +3647,8 @@
       </c>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr"/>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G116" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="117">
@@ -3688,10 +3672,8 @@
       </c>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="inlineStr"/>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G117" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="118">
@@ -3742,10 +3724,8 @@
       </c>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G119" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="120">
@@ -3877,10 +3857,8 @@
       </c>
       <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G124" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="125">
@@ -4043,10 +4021,8 @@
       </c>
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G130" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="131">
@@ -4099,10 +4075,8 @@
       </c>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G132" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="133">
@@ -4348,10 +4322,8 @@
       </c>
       <c r="E141" t="inlineStr"/>
       <c r="F141" t="inlineStr"/>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G141" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="142">
@@ -4431,10 +4403,8 @@
       </c>
       <c r="E144" t="inlineStr"/>
       <c r="F144" t="inlineStr"/>
-      <c r="G144" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G144" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="145">
@@ -4459,7 +4429,7 @@
       <c r="E145" t="inlineStr"/>
       <c r="F145" t="inlineStr"/>
       <c r="G145" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -4539,10 +4509,8 @@
       </c>
       <c r="E148" t="inlineStr"/>
       <c r="F148" t="inlineStr"/>
-      <c r="G148" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G148" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="149">
@@ -4711,10 +4679,8 @@
       </c>
       <c r="E154" t="inlineStr"/>
       <c r="F154" t="inlineStr"/>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G154" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="155">
@@ -4960,8 +4926,10 @@
       </c>
       <c r="E163" t="inlineStr"/>
       <c r="F163" t="inlineStr"/>
-      <c r="G163" t="n">
-        <v>3</v>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>Undefined</t>
+        </is>
       </c>
     </row>
     <row r="164">
@@ -5012,10 +4980,8 @@
       </c>
       <c r="E165" t="inlineStr"/>
       <c r="F165" t="inlineStr"/>
-      <c r="G165" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G165" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="166">
@@ -5039,10 +5005,8 @@
       </c>
       <c r="E166" t="inlineStr"/>
       <c r="F166" t="inlineStr"/>
-      <c r="G166" t="inlineStr">
-        <is>
-          <t>Undefined</t>
-        </is>
+      <c r="G166" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="167">

</xml_diff>